<commit_message>
Questions solved before 31 July.
</commit_message>
<xml_diff>
--- a/DailyRoutine.xlsx
+++ b/DailyRoutine.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A536A08-4BDA-4CAA-B24E-BB1521807742}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06320B69-D4C4-4AD3-9EBA-21ACF2CEE61F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{DD949E87-76F8-4E42-9465-422EE64D72B6}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="8">
   <si>
     <t>Date</t>
   </si>
@@ -34,6 +34,21 @@
   </si>
   <si>
     <t>+</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>Y</t>
   </si>
 </sst>
 </file>
@@ -401,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93C9FAFB-D9A9-4AF6-82B7-29381AD97A37}">
-  <dimension ref="A1:T418"/>
+  <dimension ref="A1:W418"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="T12" sqref="T12"/>
+    <sheetView tabSelected="1" topLeftCell="D2" workbookViewId="0">
+      <selection activeCell="T21" sqref="T21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -414,7 +429,7 @@
     <col min="19" max="19" width="10.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:23" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -475,8 +490,17 @@
       <c r="T1" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>45086</v>
       </c>
@@ -538,7 +562,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>45087</v>
       </c>
@@ -564,7 +588,7 @@
       <c r="S3" s="4"/>
       <c r="T3" s="3"/>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>45088</v>
       </c>
@@ -626,7 +650,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>45089</v>
       </c>
@@ -688,7 +712,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>45090</v>
       </c>
@@ -750,7 +774,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>45091</v>
       </c>
@@ -812,7 +836,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>45092</v>
       </c>
@@ -874,7 +898,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>45095</v>
       </c>
@@ -936,7 +960,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>45096</v>
       </c>
@@ -998,7 +1022,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>45097</v>
       </c>
@@ -1060,28 +1084,69 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
-      <c r="M12" s="3"/>
-      <c r="N12" s="3"/>
-      <c r="O12" s="3"/>
-      <c r="P12" s="3"/>
-      <c r="Q12" s="3"/>
-      <c r="R12" s="3"/>
-      <c r="S12" s="3"/>
-      <c r="T12" s="3"/>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A12" s="1">
+        <v>45099</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="M12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="N12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="O12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="P12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="R12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="S12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="T12" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.35">
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
@@ -1102,49 +1167,152 @@
       <c r="S13" s="3"/>
       <c r="T13" s="3"/>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
-      <c r="L14" s="3"/>
-      <c r="M14" s="3"/>
-      <c r="N14" s="3"/>
-      <c r="O14" s="3"/>
-      <c r="P14" s="3"/>
-      <c r="Q14" s="3"/>
-      <c r="R14" s="3"/>
-      <c r="S14" s="3"/>
-      <c r="T14" s="3"/>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="3"/>
-      <c r="L15" s="3"/>
-      <c r="M15" s="3"/>
-      <c r="N15" s="3"/>
-      <c r="O15" s="3"/>
-      <c r="P15" s="3"/>
-      <c r="Q15" s="3"/>
-      <c r="R15" s="3"/>
-      <c r="S15" s="3"/>
-      <c r="T15" s="3"/>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A14" s="1">
+        <v>45108</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K14" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="L14" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="M14" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="N14" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="O14" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="P14" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q14" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="R14" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="S14" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="T14" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="U14">
+        <v>0</v>
+      </c>
+      <c r="V14">
+        <v>1</v>
+      </c>
+      <c r="W14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A15" s="1">
+        <v>45121</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K15" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="L15" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="M15" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="N15" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="O15" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="P15" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q15" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="R15" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="S15" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="T15" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="U15">
+        <v>3</v>
+      </c>
+      <c r="V15">
+        <v>0</v>
+      </c>
+      <c r="W15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A16" s="1">
+        <v>45122</v>
+      </c>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
@@ -1164,113 +1332,372 @@
       <c r="R16" s="3"/>
       <c r="S16" s="3"/>
       <c r="T16" s="3"/>
-    </row>
-    <row r="17" spans="2:20" x14ac:dyDescent="0.35">
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
-      <c r="L17" s="3"/>
-      <c r="M17" s="3"/>
-      <c r="N17" s="3"/>
-      <c r="O17" s="3"/>
-      <c r="P17" s="3"/>
-      <c r="Q17" s="3"/>
-      <c r="R17" s="3"/>
-      <c r="S17" s="3"/>
-      <c r="T17" s="3"/>
-    </row>
-    <row r="18" spans="2:20" x14ac:dyDescent="0.35">
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
-      <c r="L18" s="3"/>
-      <c r="M18" s="3"/>
-      <c r="N18" s="3"/>
-      <c r="O18" s="3"/>
-      <c r="P18" s="3"/>
-      <c r="Q18" s="3"/>
-      <c r="R18" s="3"/>
-      <c r="S18" s="3"/>
-      <c r="T18" s="3"/>
-    </row>
-    <row r="19" spans="2:20" x14ac:dyDescent="0.35">
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
-      <c r="K19" s="3"/>
-      <c r="L19" s="3"/>
-      <c r="M19" s="3"/>
-      <c r="N19" s="3"/>
-      <c r="O19" s="3"/>
-      <c r="P19" s="3"/>
-      <c r="Q19" s="3"/>
-      <c r="R19" s="3"/>
-      <c r="S19" s="3"/>
-      <c r="T19" s="3"/>
-    </row>
-    <row r="20" spans="2:20" x14ac:dyDescent="0.35">
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
-      <c r="K20" s="3"/>
-      <c r="L20" s="3"/>
-      <c r="M20" s="3"/>
-      <c r="N20" s="3"/>
-      <c r="O20" s="3"/>
-      <c r="P20" s="3"/>
-      <c r="Q20" s="3"/>
-      <c r="R20" s="3"/>
-      <c r="S20" s="3"/>
-      <c r="T20" s="3"/>
-    </row>
-    <row r="21" spans="2:20" x14ac:dyDescent="0.35">
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
-      <c r="K21" s="3"/>
-      <c r="L21" s="3"/>
-      <c r="M21" s="3"/>
-      <c r="N21" s="3"/>
-      <c r="O21" s="3"/>
-      <c r="P21" s="3"/>
-      <c r="Q21" s="3"/>
-      <c r="R21" s="3"/>
-      <c r="S21" s="3"/>
-      <c r="T21" s="3"/>
-    </row>
-    <row r="22" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="U16">
+        <v>0</v>
+      </c>
+      <c r="V16">
+        <v>1</v>
+      </c>
+      <c r="W16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A17" s="1">
+        <v>45123</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K17" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="L17" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="M17" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="N17" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="O17" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="P17" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q17" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="R17" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="S17" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="T17" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="U17">
+        <v>1</v>
+      </c>
+      <c r="V17">
+        <v>1</v>
+      </c>
+      <c r="W17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A18" s="1">
+        <v>45124</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K18" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="L18" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="M18" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="N18" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="O18" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="P18" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q18" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="R18" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="S18" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="T18" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="U18">
+        <v>0</v>
+      </c>
+      <c r="V18">
+        <v>0</v>
+      </c>
+      <c r="W18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A19" s="1">
+        <v>45125</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K19" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="L19" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="M19" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="N19" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="O19" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="P19" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q19" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="R19" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="S19" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="T19" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="U19">
+        <v>0</v>
+      </c>
+      <c r="V19">
+        <v>1</v>
+      </c>
+      <c r="W19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A20" s="1">
+        <v>45126</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K20" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="L20" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="M20" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="N20" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="O20" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="P20" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q20" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="R20" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="S20" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="T20" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="U20">
+        <v>0</v>
+      </c>
+      <c r="V20">
+        <v>1</v>
+      </c>
+      <c r="W20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A21" s="1">
+        <v>45127</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="J21" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K21" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="L21" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="M21" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="N21" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="O21" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="P21" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q21" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="R21" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="S21" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="T21" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="U21">
+        <v>0</v>
+      </c>
+      <c r="V21">
+        <v>1</v>
+      </c>
+      <c r="W21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.35">
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
@@ -1291,7 +1718,7 @@
       <c r="S22" s="3"/>
       <c r="T22" s="3"/>
     </row>
-    <row r="23" spans="2:20" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.35">
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
@@ -1312,7 +1739,7 @@
       <c r="S23" s="3"/>
       <c r="T23" s="3"/>
     </row>
-    <row r="24" spans="2:20" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.35">
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
@@ -1333,7 +1760,7 @@
       <c r="S24" s="3"/>
       <c r="T24" s="3"/>
     </row>
-    <row r="25" spans="2:20" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.35">
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
@@ -1354,7 +1781,7 @@
       <c r="S25" s="3"/>
       <c r="T25" s="3"/>
     </row>
-    <row r="26" spans="2:20" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.35">
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
@@ -1375,7 +1802,7 @@
       <c r="S26" s="3"/>
       <c r="T26" s="3"/>
     </row>
-    <row r="27" spans="2:20" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.35">
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
@@ -1396,7 +1823,7 @@
       <c r="S27" s="3"/>
       <c r="T27" s="3"/>
     </row>
-    <row r="28" spans="2:20" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.35">
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
@@ -1417,7 +1844,7 @@
       <c r="S28" s="3"/>
       <c r="T28" s="3"/>
     </row>
-    <row r="29" spans="2:20" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.35">
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
@@ -1438,7 +1865,7 @@
       <c r="S29" s="3"/>
       <c r="T29" s="3"/>
     </row>
-    <row r="30" spans="2:20" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.35">
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
@@ -1459,7 +1886,7 @@
       <c r="S30" s="3"/>
       <c r="T30" s="3"/>
     </row>
-    <row r="31" spans="2:20" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.35">
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
@@ -1480,7 +1907,7 @@
       <c r="S31" s="3"/>
       <c r="T31" s="3"/>
     </row>
-    <row r="32" spans="2:20" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.35">
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>

</xml_diff>